<commit_message>
aula do dia 25
</commit_message>
<xml_diff>
--- a/fia/20210520/dados/People_Analytics_v2.xlsx
+++ b/fia/20210520/dados/People_Analytics_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uedap\Patricia\AulasFIA\Análise Exploratória\Corrigido\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\github.com\datascience\fia\20210520\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0BA13E38-F8D1-4589-AAD7-C444CEE96689}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A26A00B-86C0-4BC0-B3F6-384193EC5010}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-465" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BaseDados" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="71">
   <si>
     <t>N</t>
   </si>
@@ -216,6 +216,39 @@
   </si>
   <si>
     <t>setwd("C:\...")</t>
+  </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Mediana</t>
+  </si>
+  <si>
+    <t>Moda</t>
+  </si>
+  <si>
+    <t>q1</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>Minimo</t>
+  </si>
+  <si>
+    <t>Maximo</t>
+  </si>
+  <si>
+    <t>q2 / Mediana</t>
   </si>
 </sst>
 </file>
@@ -834,7 +867,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -845,6 +880,7 @@
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -913,6 +949,13 @@
       <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="H3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3">
+        <f>AVERAGE(F2:F37)</f>
+        <v>34.583333333333336</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -936,6 +979,13 @@
       <c r="G4" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="H4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4">
+        <f>MEDIAN(F1:F37)</f>
+        <v>34.5</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -957,6 +1007,13 @@
       <c r="G5" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5">
+        <f>MODE(F2:F37)</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -978,6 +1035,13 @@
       <c r="G6" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="H6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6">
+        <f>_xlfn.QUARTILE.INC(F$2:F$37,1)</f>
+        <v>30</v>
+      </c>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1002,6 +1066,13 @@
       <c r="G7" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="H7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7">
+        <f>_xlfn.QUARTILE.INC(F$2:F$37,2)</f>
+        <v>34.5</v>
+      </c>
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1024,6 +1095,13 @@
       <c r="G8" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="H8" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8">
+        <f>_xlfn.QUARTILE.INC(F$2:F$37,3)</f>
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
@@ -1045,6 +1123,13 @@
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="H9" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9">
+        <f>_xlfn.QUARTILE.INC(F$2:F$37,4)</f>
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
@@ -1068,6 +1153,13 @@
       <c r="G10" s="8" t="s">
         <v>10</v>
       </c>
+      <c r="H10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I10">
+        <f>PERCENTILE(F$2:F$37,0.01)</f>
+        <v>21.05</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
@@ -1089,6 +1181,13 @@
       <c r="G11" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="H11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11">
+        <f>PERCENTILE(F$2:F$37,0.99)</f>
+        <v>47.3</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
@@ -1112,6 +1211,13 @@
       <c r="G12" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="H12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12">
+        <f>MIN(F2:F37)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
@@ -1132,6 +1238,13 @@
       </c>
       <c r="G13" s="8" t="s">
         <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>69</v>
+      </c>
+      <c r="I13">
+        <f>MAX(F2:F37)</f>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1677,13 +1790,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3D3E3EA-62FC-4F17-8989-C77CFF037EDF}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="18" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>15</v>
       </c>

</xml_diff>